<commit_message>
[Reports] Feat: style changes
</commit_message>
<xml_diff>
--- a/src/main/resources/report_template.xlsx
+++ b/src/main/resources/report_template.xlsx
@@ -503,8 +503,8 @@
   </sheetPr>
   <dimension ref="A1:AG19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J14" colorId="64" zoomScale="53" zoomScaleNormal="53" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q26" activeCellId="0" sqref="Q26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="53" zoomScaleNormal="53" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S40" activeCellId="0" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1393,62 +1393,77 @@
         <v>29</v>
       </c>
       <c r="B14" s="7" t="n">
+        <f aca="false">B8-SUM(B9:C13)</f>
         <v>0</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7" t="n">
+        <f aca="false">D8-SUM(D9:E13)</f>
         <v>0</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7" t="n">
+        <f aca="false">F8-SUM(F9:G13)</f>
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7" t="n">
+        <f aca="false">H8-SUM(H9:I13)</f>
         <v>0</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7" t="n">
+        <f aca="false">J8-SUM(J9:K13)</f>
         <v>0</v>
       </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7" t="n">
+        <f aca="false">L8-SUM(L9:M13)</f>
         <v>0</v>
       </c>
       <c r="M14" s="7"/>
       <c r="N14" s="7" t="n">
+        <f aca="false">N8-SUM(N9:O13)</f>
         <v>0</v>
       </c>
       <c r="O14" s="7"/>
       <c r="P14" s="7" t="n">
+        <f aca="false">P8-SUM(P9:Q13)</f>
         <v>0</v>
       </c>
       <c r="Q14" s="7"/>
       <c r="R14" s="7" t="n">
+        <f aca="false">R8-SUM(R9:S13)</f>
         <v>0</v>
       </c>
       <c r="S14" s="7"/>
       <c r="T14" s="7" t="n">
+        <f aca="false">T8-SUM(T9:U13)</f>
         <v>0</v>
       </c>
       <c r="U14" s="7"/>
       <c r="V14" s="7" t="n">
+        <f aca="false">V8-SUM(V9:W13)</f>
         <v>0</v>
       </c>
       <c r="W14" s="7"/>
       <c r="X14" s="7" t="n">
+        <f aca="false">X8-SUM(X9:Y13)</f>
         <v>0</v>
       </c>
       <c r="Y14" s="7"/>
       <c r="Z14" s="7" t="n">
+        <f aca="false">Z8-SUM(Z9:AA13)</f>
         <v>0</v>
       </c>
       <c r="AA14" s="7"/>
       <c r="AB14" s="7" t="n">
+        <f aca="false">AB8-SUM(AB9:AC13)</f>
         <v>0</v>
       </c>
       <c r="AC14" s="7"/>
       <c r="AD14" s="7" t="n">
+        <f aca="false">AD8-SUM(AD9:AE13)</f>
         <v>0</v>
       </c>
       <c r="AE14" s="7"/>
@@ -1743,62 +1758,77 @@
         <v>34</v>
       </c>
       <c r="B19" s="7" t="n">
+        <f aca="false">B15-SUM(B16:C18)</f>
         <v>0</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="n">
+        <f aca="false">D15-SUM(D16:E18)</f>
         <v>0</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7" t="n">
+        <f aca="false">F15-SUM(F16:G18)</f>
         <v>0</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7" t="n">
+        <f aca="false">H15-SUM(H16:I18)</f>
         <v>0</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7" t="n">
+        <f aca="false">J15-SUM(J16:K18)</f>
         <v>0</v>
       </c>
       <c r="K19" s="7"/>
       <c r="L19" s="7" t="n">
+        <f aca="false">L15-SUM(L16:M18)</f>
         <v>0</v>
       </c>
       <c r="M19" s="7"/>
       <c r="N19" s="7" t="n">
+        <f aca="false">N15-SUM(N16:O18)</f>
         <v>0</v>
       </c>
       <c r="O19" s="7"/>
       <c r="P19" s="7" t="n">
+        <f aca="false">P15-SUM(P16:Q18)</f>
         <v>0</v>
       </c>
       <c r="Q19" s="7"/>
       <c r="R19" s="7" t="n">
+        <f aca="false">R15-SUM(R16:S18)</f>
         <v>0</v>
       </c>
       <c r="S19" s="7"/>
       <c r="T19" s="7" t="n">
+        <f aca="false">T15-SUM(T16:U18)</f>
         <v>0</v>
       </c>
       <c r="U19" s="7"/>
       <c r="V19" s="7" t="n">
+        <f aca="false">V15-SUM(V16:W18)</f>
         <v>0</v>
       </c>
       <c r="W19" s="7"/>
       <c r="X19" s="7" t="n">
+        <f aca="false">X15-SUM(X16:Y18)</f>
         <v>0</v>
       </c>
       <c r="Y19" s="7"/>
       <c r="Z19" s="7" t="n">
+        <f aca="false">Z15-SUM(Z16:AA18)</f>
         <v>0</v>
       </c>
       <c r="AA19" s="7"/>
       <c r="AB19" s="7" t="n">
+        <f aca="false">AB15-SUM(AB16:AC18)</f>
         <v>0</v>
       </c>
       <c r="AC19" s="7"/>
       <c r="AD19" s="7" t="n">
+        <f aca="false">AD15-SUM(AD16:AE18)</f>
         <v>0</v>
       </c>
       <c r="AE19" s="7"/>

</xml_diff>